<commit_message>
Working validation of version
</commit_message>
<xml_diff>
--- a/uploads/123-template-2018-03-26.xlsx
+++ b/uploads/123-template-2018-03-26.xlsx
@@ -11,114 +11,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>PF CLUB NAME 1</t>
+  </si>
+  <si>
+    <t>PF CLUB NAME 2</t>
+  </si>
+  <si>
+    <t>PF CLUB NAME 3</t>
+  </si>
+  <si>
+    <t>PF CLUB NAME 4</t>
+  </si>
+  <si>
+    <t>PF CLUB NAME 5</t>
+  </si>
+  <si>
+    <t>PF CLUB NAME 6</t>
+  </si>
+  <si>
+    <t>Tactic</t>
+  </si>
+  <si>
+    <t>PF Club Id 1</t>
+  </si>
+  <si>
+    <t>PF Club Id 2</t>
+  </si>
+  <si>
+    <t>PF Club Id 3</t>
+  </si>
+  <si>
+    <t>PF Club Id 4</t>
+  </si>
+  <si>
+    <t>PF Club Id 5</t>
+  </si>
+  <si>
+    <t>PF Club Id 6</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>Streaming Television</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Streaming Radio</t>
+  </si>
+  <si>
+    <t>Direct Mail</t>
+  </si>
+  <si>
+    <t>Shared Mail</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Digital Display</t>
+  </si>
+  <si>
+    <t>SEO/SEM</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>OOH</t>
+  </si>
+  <si>
+    <t>Newspaper</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Sponsorship(s)</t>
+  </si>
+  <si>
+    <t>Guerilla Marketing</t>
+  </si>
+  <si>
+    <t>Promotional POP</t>
+  </si>
+  <si>
+    <t>Public Relations Fee</t>
+  </si>
+  <si>
+    <t>Production Fees</t>
+  </si>
+  <si>
+    <t>Agency Fees</t>
+  </si>
+  <si>
+    <t>Reoccurring Co-Op Contribution</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>PF CLUB NAME 1</t>
-  </si>
-  <si>
-    <t>PF CLUB NAME 2</t>
-  </si>
-  <si>
-    <t>PF CLUB NAME 3</t>
-  </si>
-  <si>
-    <t>PF CLUB NAME 4</t>
-  </si>
-  <si>
-    <t>PF CLUB NAME 5</t>
-  </si>
-  <si>
-    <t>PF CLUB NAME 6</t>
-  </si>
-  <si>
-    <t>Tactic</t>
-  </si>
-  <si>
-    <t>PF Club Id 1</t>
-  </si>
-  <si>
-    <t>PF Club Id 2</t>
-  </si>
-  <si>
-    <t>PF Club Id 3</t>
-  </si>
-  <si>
-    <t>PF Club Id 4</t>
-  </si>
-  <si>
-    <t>PF Club Id 5</t>
-  </si>
-  <si>
-    <t>PF Club Id 6</t>
-  </si>
-  <si>
-    <t>Television</t>
-  </si>
-  <si>
-    <t>Streaming Television</t>
-  </si>
-  <si>
-    <t>Radio</t>
-  </si>
-  <si>
-    <t>Streaming Radio</t>
-  </si>
-  <si>
-    <t>Direct Mail</t>
-  </si>
-  <si>
-    <t>Shared Mail</t>
-  </si>
-  <si>
-    <t>Letter</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Digital Display</t>
-  </si>
-  <si>
-    <t>SEO/SEM</t>
-  </si>
-  <si>
-    <t>Social</t>
-  </si>
-  <si>
-    <t>OOH</t>
-  </si>
-  <si>
-    <t>Newspaper</t>
-  </si>
-  <si>
-    <t>Events</t>
-  </si>
-  <si>
-    <t>Sponsorship(s)</t>
-  </si>
-  <si>
-    <t>Guerilla Marketing</t>
-  </si>
-  <si>
-    <t>Promotional POP</t>
-  </si>
-  <si>
-    <t>Public Relations Fee</t>
-  </si>
-  <si>
-    <t>Production Fees</t>
-  </si>
-  <si>
-    <t>Agency Fees</t>
-  </si>
-  <si>
-    <t>Reoccurring Co-Op Contribution</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Promotional Club Expense</t>
@@ -550,54 +550,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
+      <c r="A1" s="4">
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="9">
         <f>SUM(B3:B23)</f>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>